<commit_message>
Atualizando o tabelas do banco de dados
</commit_message>
<xml_diff>
--- a/leads.xlsx
+++ b/leads.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,6 +664,43 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Leonardo</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fragoso</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>LeoFragoso</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>21980292791</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>leonardorfragoso@gmail.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Igual este</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>